<commit_message>
commit con fe bcp
</commit_message>
<xml_diff>
--- a/res/nueva base solicitudes 2018-2.xlsx
+++ b/res/nueva base solicitudes 2018-2.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SGRU_laravel\res\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
   <si>
     <t>Código</t>
   </si>
@@ -108,8 +113,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -303,7 +308,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -480,27 +485,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -552,7 +557,7 @@
         <v>42919</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -569,7 +574,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="5">
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>23</v>
@@ -578,7 +583,7 @@
         <v>42919</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -593,7 +598,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5">
-        <v>43102</v>
+        <v>43104</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>23</v>
@@ -602,7 +607,7 @@
         <v>42947</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -619,7 +624,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="5">
-        <v>43102</v>
+        <v>43105</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>23</v>
@@ -628,7 +633,7 @@
         <v>42947</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>999999</v>
       </c>
@@ -652,7 +657,7 @@
         <v>42947</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>999999</v>
       </c>
@@ -678,7 +683,7 @@
         <v>42949</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>999999</v>
       </c>
@@ -704,7 +709,7 @@
         <v>42920</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>999999</v>
       </c>
@@ -730,7 +735,7 @@
         <v>42922</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>999999</v>
       </c>
@@ -747,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="5">
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>23</v>
@@ -756,7 +761,7 @@
         <v>42917</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>888888</v>
       </c>
@@ -773,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="5">
-        <v>43102</v>
+        <v>43104</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>23</v>
@@ -782,7 +787,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>888888</v>
       </c>
@@ -808,7 +813,7 @@
         <v>42920</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>888888</v>
       </c>
@@ -834,7 +839,7 @@
         <v>42926</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>888888</v>
       </c>
@@ -851,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="5">
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>23</v>
@@ -860,7 +865,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>888888</v>
       </c>
@@ -877,7 +882,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="5">
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>23</v>
@@ -886,7 +891,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>888888</v>
       </c>
@@ -903,7 +908,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="5">
-        <v>43102</v>
+        <v>43103</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>23</v>
@@ -912,7 +917,7 @@
         <v>42921</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>888888</v>
       </c>
@@ -929,7 +934,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="5">
-        <v>43102</v>
+        <v>43104</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>23</v>
@@ -938,7 +943,7 @@
         <v>42919</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>888888</v>
       </c>
@@ -955,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="5">
-        <v>43102</v>
+        <v>43105</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>23</v>
@@ -964,7 +969,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>888888</v>
       </c>
@@ -990,7 +995,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>888888</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>42949</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>888888</v>
       </c>
@@ -1040,6 +1045,50 @@
       </c>
       <c r="H21" s="6">
         <v>42950</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4">
+        <v>923456</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="5">
+        <v>43102</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="6">
+        <v>42919</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="4">
+        <v>923457</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="5">
+        <v>43102</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="6">
+        <v>42919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>